<commit_message>
Added Kling-Gupta efficiency to statistics.py
</commit_message>
<xml_diff>
--- a/tests/test6/cotton2022p10-2_fitdata.xlsx
+++ b/tests/test6/cotton2022p10-2_fitdata.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mnt\Data1\USDA-ALARC\Simulation Modeling\FAO56\pyfao56\tests\test6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{70208FA6-C735-4EAF-B895-781EEF563299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D031FF-E336-435B-84B7-2E95096DFB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3330" yWindow="-25890" windowWidth="16290" windowHeight="17910"/>
+    <workbookView xWindow="16965" yWindow="-22410" windowWidth="17340" windowHeight="21300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dr" sheetId="1" r:id="rId1"/>
     <sheet name="Drmax" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>sDr</t>
   </si>
@@ -116,11 +129,17 @@
   <si>
     <t>meanerr</t>
   </si>
+  <si>
+    <t>kge</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,7 +619,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -660,9 +679,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -700,7 +719,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -806,7 +825,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -948,24 +967,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -988,7 +1011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>27.1999999999998</v>
       </c>
@@ -1008,7 +1031,7 @@
         <v>120.95798364864767</v>
       </c>
       <c r="F2">
-        <f>(B2-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" ref="F2:F26" si="0">(B2-AVERAGE(B$2:B$26))^2</f>
         <v>5114.6289386184926</v>
       </c>
       <c r="G2">
@@ -1016,35 +1039,35 @@
         <v>17433.288229221231</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>13.684522746741299</v>
+        <v>15.6494878213382</v>
       </c>
       <c r="B3" s="1">
         <v>11.599420000023301</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C26" si="0">(A3-B3)</f>
-        <v>2.0851027467179986</v>
+        <f t="shared" ref="C3:C26" si="1">(A3-B3)</f>
+        <v>4.0500678213148991</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D26" si="1">ABS(C3)</f>
-        <v>2.0851027467179986</v>
+        <f t="shared" ref="D3:D26" si="2">ABS(C3)</f>
+        <v>4.0500678213148991</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E26" si="2">C3*C3</f>
-        <v>4.3476534643709419</v>
+        <f t="shared" ref="E3:E26" si="3">C3*C3</f>
+        <v>16.403049357250413</v>
       </c>
       <c r="F3">
-        <f>(B3-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>2017.6234898602856</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G26" si="3">(ABS(A3-AVERAGE($B$2:$B$26))+ABS(B3-AVERAGE($B$2:$B$26)))^2</f>
-        <v>8449.4758933548546</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" ref="G3:G26" si="4">(ABS(A3-AVERAGE($B$2:$B$26))+ABS(B3-AVERAGE($B$2:$B$26)))^2</f>
+        <v>8814.5802111718003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>13.0893405284962</v>
       </c>
@@ -1052,775 +1075,784 @@
         <v>6.1996900000160897</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8896505284801099</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8896505284801099</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47.467284404586259</v>
       </c>
       <c r="F4">
-        <f>(B4-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1561.6908184385868</v>
       </c>
       <c r="G4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7383.2978451957306</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>13.281382672687499</v>
+        <v>14.7448891462071</v>
       </c>
       <c r="B5" s="1">
         <v>5.1997400000282603</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>8.081642672659239</v>
+        <f t="shared" si="1"/>
+        <v>9.54514914617884</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>8.081642672659239</v>
+        <f t="shared" si="2"/>
+        <v>9.54514914617884</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>65.312948288546764</v>
+        <f t="shared" si="3"/>
+        <v>91.109872222798643</v>
       </c>
       <c r="F5">
-        <f>(B5-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1483.6582022664409</v>
       </c>
       <c r="G5">
-        <f t="shared" si="3"/>
-        <v>7245.1097879463032</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>7496.393743809117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>12.040360120451499</v>
+        <v>15.6466964913062</v>
       </c>
       <c r="B6" s="1">
         <v>6.1996900000160897</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>5.8406701204354095</v>
+        <f t="shared" si="1"/>
+        <v>9.4470064912901108</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>5.8406701204354095</v>
+        <f t="shared" si="2"/>
+        <v>9.4470064912901108</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>34.113427455746979</v>
+        <f t="shared" si="3"/>
+        <v>89.245931646477487</v>
       </c>
       <c r="F6">
-        <f>(B6-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1561.6908184385868</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
-        <v>7204.1285753429183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>7829.3252578709053</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>16.546944111758599</v>
+        <v>21.5910927482043</v>
       </c>
       <c r="B7" s="1">
         <v>6.5837900000061698</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>9.9631541117524289</v>
+        <f t="shared" si="1"/>
+        <v>15.00730274819813</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>9.9631541117524289</v>
+        <f t="shared" si="2"/>
+        <v>15.00730274819813</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>99.264439854529328</v>
+        <f t="shared" si="3"/>
+        <v>225.21913577607515</v>
       </c>
       <c r="F7">
-        <f>(B7-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1592.1962586062043</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
-        <v>8058.2618865011718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>8989.3097969606661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6.8296693569677096</v>
+        <v>9.1314260373540002</v>
       </c>
       <c r="B8" s="1">
         <v>7.9401099998860696</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>-1.11044064291836</v>
+        <f t="shared" si="1"/>
+        <v>1.1913160374679306</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>1.11044064291836</v>
+        <f t="shared" si="2"/>
+        <v>1.1913160374679306</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>1.2330784214449406</v>
+        <f t="shared" si="3"/>
+        <v>1.4192339011282917</v>
       </c>
       <c r="F8">
-        <f>(B8-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1702.2765298390486</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
-        <v>6627.0780526856488</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>7007.1337380324421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>18.2981383951387</v>
+        <v>19.432721010301101</v>
       </c>
       <c r="B9" s="1">
         <v>4.4706500001344898</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>13.82748839500421</v>
+        <f t="shared" si="1"/>
+        <v>14.962071010166611</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>13.82748839500421</v>
+        <f t="shared" si="2"/>
+        <v>14.962071010166611</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>191.1994353139761</v>
+        <f t="shared" si="3"/>
+        <v>223.8635689132681</v>
       </c>
       <c r="F9">
-        <f>(B9-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1428.0231831401727</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
-        <v>7993.4107338193562</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>8197.5747176304758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>22.1225426696402</v>
+        <v>22.5216586248869</v>
       </c>
       <c r="B10" s="1">
         <v>-12.647820000043801</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>34.770362669684005</v>
+        <f t="shared" si="1"/>
+        <v>35.169478624930704</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>34.770362669684005</v>
+        <f t="shared" si="2"/>
+        <v>35.169478624930704</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>1208.9781201813551</v>
+        <f t="shared" si="3"/>
+        <v>1236.8922267494577</v>
       </c>
       <c r="F10">
-        <f>(B10-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>427.27883066068875</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
-        <v>5793.0077232448584</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>5853.9218928316577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>12.8066560959927</v>
+        <v>13.283504509425301</v>
       </c>
       <c r="B11" s="1">
         <v>-38.051819999574498</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>50.858476095567198</v>
+        <f t="shared" si="1"/>
+        <v>51.335324508999797</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>50.858476095567198</v>
+        <f t="shared" si="2"/>
+        <v>51.335324508999797</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>2586.5845907633802</v>
+        <f t="shared" si="3"/>
+        <v>2635.3155424443153</v>
       </c>
       <c r="F11">
-        <f>(B11-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>22.403901693111539</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
-        <v>2586.5845907633802</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>2635.3155424443153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>24.562731439754501</v>
+        <v>24.951864233187901</v>
       </c>
       <c r="B12" s="1">
         <v>-58.546359999903302</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>83.109091439657803</v>
+        <f t="shared" si="1"/>
+        <v>83.498224233091207</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>83.109091439657803</v>
+        <f t="shared" si="2"/>
+        <v>83.498224233091207</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>6907.1210799254022</v>
+        <f t="shared" si="3"/>
+        <v>6971.9534500795799</v>
       </c>
       <c r="F12">
-        <f>(B12-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>636.4427001514324</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
-        <v>6907.1210799254022</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>6971.9534500795799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>21.269594282810299</v>
+        <v>21.663315873935701</v>
       </c>
       <c r="B13" s="1">
         <v>-62.118479998901996</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>83.388074281712292</v>
+        <f t="shared" si="1"/>
+        <v>83.781795872837705</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>83.388074281712292</v>
+        <f t="shared" si="2"/>
+        <v>83.781795872837705</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
-        <v>6953.5709324123673</v>
+        <f t="shared" si="3"/>
+        <v>7019.3893196778454</v>
       </c>
       <c r="F13">
-        <f>(B13-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>829.43631357105232</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
-        <v>6953.5709324123673</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>7019.3893196778454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>17.4831133695061</v>
+        <v>17.633116728369501</v>
       </c>
       <c r="B14" s="1">
         <v>-63.299269999521897</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>80.782383369027997</v>
+        <f t="shared" si="1"/>
+        <v>80.932386727891398</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>80.782383369027997</v>
+        <f t="shared" si="2"/>
+        <v>80.932386727891398</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
-        <v>6525.7934627806108</v>
+        <f t="shared" si="3"/>
+        <v>6550.0512214729715</v>
       </c>
       <c r="F14">
-        <f>(B14-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>898.84393148984771</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
-        <v>6525.7934627806108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>6550.0512214729715</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>15.8542831263943</v>
+        <v>15.8556917152879</v>
       </c>
       <c r="B15" s="1">
         <v>-63.599199999314401</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>79.453483125708701</v>
+        <f t="shared" si="1"/>
+        <v>79.454891714602297</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>79.453483125708701</v>
+        <f t="shared" si="2"/>
+        <v>79.454891714602297</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
-        <v>6312.8559808072769</v>
+        <f t="shared" si="3"/>
+        <v>6313.0798173791763</v>
       </c>
       <c r="F15">
-        <f>(B15-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>916.91812778056919</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
-        <v>6312.8559808072769</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>6313.0798173791763</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>20.0066875678922</v>
+        <v>20.188900431782901</v>
       </c>
       <c r="B16" s="1">
         <v>-66.599219999403203</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>86.605907567295404</v>
+        <f t="shared" si="1"/>
+        <v>86.788120431186101</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>86.605907567295404</v>
+        <f t="shared" si="2"/>
+        <v>86.788120431186101</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
-        <v>7500.5832255549149</v>
+        <f t="shared" si="3"/>
+        <v>7532.1778479780623</v>
       </c>
       <c r="F16">
-        <f>(B16-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1107.6033950121523</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
-        <v>7500.5832255549149</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>7532.1778479780651</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>17.21878422372</v>
+        <v>17.152638564649799</v>
       </c>
       <c r="B17" s="1">
         <v>-76.799179999169596</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>94.017964222889589</v>
+        <f t="shared" si="1"/>
+        <v>93.951818563819387</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>94.017964222889589</v>
+        <f t="shared" si="2"/>
+        <v>93.951818563819387</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
-        <v>8839.3775966165467</v>
+        <f t="shared" si="3"/>
+        <v>8826.9442114488375</v>
       </c>
       <c r="F17">
-        <f>(B17-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1890.5657069378792</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
-        <v>8839.3775966165467</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>8826.9442114488375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>12.594250000000001</v>
+        <v>12.5793083442318</v>
       </c>
       <c r="B18" s="1">
         <v>-71.399239999576807</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>83.993489999576809</v>
+        <f t="shared" si="1"/>
+        <v>83.978548343808612</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>83.993489999576809</v>
+        <f t="shared" si="2"/>
+        <v>83.978548343808612</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
-        <v>7054.9063623090096</v>
+        <f t="shared" si="3"/>
+        <v>7052.3965819333998</v>
       </c>
       <c r="F18">
-        <f>(B18-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1450.1394078521187</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
-        <v>7054.9063623090096</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>7052.396581933398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>16.554566004815101</v>
+        <v>16.546550488609601</v>
       </c>
       <c r="B19" s="1">
         <v>-83.599159998864806</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>100.15372600367991</v>
+        <f t="shared" si="1"/>
+        <v>100.1457104874744</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>100.15372600367991</v>
+        <f t="shared" si="2"/>
+        <v>100.1457104874744</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
-        <v>10030.768832420188</v>
+        <f t="shared" si="3"/>
+        <v>10029.163329041041</v>
       </c>
       <c r="F19">
-        <f>(B19-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>2528.1403452780264</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
-        <v>10030.768832420188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>10029.163329041043</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>30.005727805739902</v>
+        <v>30.2881972794024</v>
       </c>
       <c r="B20" s="1">
         <v>-65.799219998663801</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>95.804947804403696</v>
+        <f t="shared" si="1"/>
+        <v>96.087417278066198</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
-        <v>95.804947804403696</v>
+        <f t="shared" si="2"/>
+        <v>96.087417278066198</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
-        <v>9178.5880238045174</v>
+        <f t="shared" si="3"/>
+        <v>9232.7917591692149</v>
       </c>
       <c r="F20">
-        <f>(B20-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1054.9943133642357</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
-        <v>9178.5880238045174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>9232.7917591692149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>7.30497160240576</v>
+        <v>7.2509557459792404</v>
       </c>
       <c r="B21" s="1">
         <v>-88.6992899993934</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>96.004261601799158</v>
+        <f t="shared" si="1"/>
+        <v>95.950245745372641</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>96.004261601799158</v>
+        <f t="shared" si="2"/>
+        <v>95.950245745372641</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
-        <v>9216.8182457066887</v>
+        <f t="shared" si="3"/>
+        <v>9206.4496585974011</v>
       </c>
       <c r="F21">
-        <f>(B21-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>3067.0270275074035</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
-        <v>9216.8182457066887</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>9206.4496585974011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>45.312769420289101</v>
+        <v>46.187126821272102</v>
       </c>
       <c r="B22" s="1">
         <v>-45.399359998297697</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>90.712129418586798</v>
+        <f t="shared" si="1"/>
+        <v>91.586486819569799</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
-        <v>90.712129418586798</v>
+        <f t="shared" si="2"/>
+        <v>91.586486819569799</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
-        <v>8228.6904236544397</v>
+        <f t="shared" si="3"/>
+        <v>8388.0845679512331</v>
       </c>
       <c r="F22">
-        <f>(B22-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>145.94611519739422</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
-        <v>8228.6904236544433</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>8388.0845679512349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>54.870090874615798</v>
+        <v>56.491329067400102</v>
       </c>
       <c r="B23" s="1">
         <v>-55.799199999449101</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>110.6692908740649</v>
+        <f t="shared" si="1"/>
+        <v>112.2905290668492</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
-        <v>110.6692908740649</v>
+        <f t="shared" si="2"/>
+        <v>112.2905290668492</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
-        <v>12247.691942568385</v>
+        <f t="shared" si="3"/>
+        <v>12609.162918112906</v>
       </c>
       <c r="F23">
-        <f>(B23-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>505.37989418914134</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
-        <v>12247.691942568385</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>12609.162918112908</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>103.64004406186901</v>
+        <v>105.779654445178</v>
       </c>
       <c r="B24" s="1">
         <v>-15.6992899989924</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>119.3393340608614</v>
+        <f t="shared" si="1"/>
+        <v>121.47894444417039</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
-        <v>119.3393340608614</v>
+        <f t="shared" si="2"/>
+        <v>121.47894444417039</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
-        <v>14241.876654089874</v>
+        <f t="shared" si="3"/>
+        <v>14757.133943269837</v>
       </c>
       <c r="F24">
-        <f>(B24-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>310.43811153354585</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
-        <v>23894.309256491422</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>24560.359900893756</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>111.133312213243</v>
+        <v>114.747292581568</v>
       </c>
       <c r="B25" s="1">
         <v>-23.099309998818899</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>134.2326222120619</v>
+        <f t="shared" si="1"/>
+        <v>137.8466025803869</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
-        <v>134.2326222120619</v>
+        <f t="shared" si="2"/>
+        <v>137.8466025803869</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
-        <v>18018.396865926134</v>
+        <f t="shared" si="3"/>
+        <v>19001.685842955128</v>
       </c>
       <c r="F25">
-        <f>(B25-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>104.43274356017943</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
-        <v>23923.146147794123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>25054.16356905389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>119.23831221324301</v>
+        <v>122.857960757832</v>
       </c>
       <c r="B26" s="1">
         <v>-28.1993599991374</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>147.43767221238039</v>
+        <f t="shared" si="1"/>
+        <v>151.0573207569694</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
-        <v>147.43767221238039</v>
+        <f t="shared" si="2"/>
+        <v>151.0573207569694</v>
       </c>
       <c r="E26">
-        <f t="shared" si="2"/>
-        <v>21737.867187405325</v>
+        <f t="shared" si="3"/>
+        <v>22818.314154273939</v>
       </c>
       <c r="F26">
-        <f>(B26-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>26.206044829319357</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
-        <v>24861.733657269553</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>26016.299211803387</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
         <f>SUM(C2:C26)</f>
-        <v>1605.9123948910642</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1635.4283199830977</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30">
         <f>SUM(C2:C26)/AVERAGE(B2:B26)</f>
-        <v>-48.198756671850248</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-49.084627467779931</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31">
         <f>SUM(C2:C26)/AVERAGE(B2:B26)*100</f>
-        <v>-4819.8756671850251</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-4908.4627467779928</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32" cm="1">
         <f t="array" ref="B32">MAX(ABS(C2:C26))</f>
-        <v>147.43767221238039</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>151.0573207569694</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
       <c r="B33">
         <f>AVERAGE(C2:C26)</f>
-        <v>64.236495795642568</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>65.417132799323909</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34">
         <f>AVERAGE(D2:D26)</f>
-        <v>65.205178247078024</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>66.296979999325899</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
       <c r="B35">
         <f>SUM(E2:E26)</f>
-        <v>157354.36577777826</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>160996.67245240457</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
       <c r="B36">
         <f>CORREL(A2:A26,B2:B26)</f>
-        <v>5.4369197740728223E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7.5405467076032101E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
       <c r="B37">
         <f>B36^2</f>
-        <v>2.9560096629704068E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5.6859844649545608E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="B38">
         <f>SQRT(AVERAGE(E2:E26))</f>
-        <v>79.335834470377449</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>80.248781287295472</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
       <c r="B39">
         <f>B38/AVERAGE(B2:B26)</f>
-        <v>-2.3811314945702891</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-2.408532056159427</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
       <c r="B40">
         <f>B39*100</f>
-        <v>-238.1131494570289</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-240.8532056159427</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
       <c r="B41">
         <f>(SUM(A2:A26)-SUM(B2:B26))/SUM(B2:B26)</f>
-        <v>-1.9279502668740101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-1.9633850987111974</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
       <c r="B42">
         <f>1-SUM(E2:E26)/SUM(F2:F26)</f>
-        <v>-3.8590179698335465</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-3.9714904360163263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
       <c r="B43">
         <f>1-SUM(E2:E26)/SUM(G2:G26)</f>
-        <v>0.3717124454276266</v>
+        <v>0.37356016153904292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44">
+        <f>1-SQRT((B36-1)^2+(STDEV(A2:A26)/STDEV(B2:B26)-1)^2+(AVERAGE(A2:A26)/AVERAGE(B2:B26)-1)^2)</f>
+        <v>-1.1726830669481414</v>
       </c>
     </row>
   </sheetData>
@@ -1829,14 +1861,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1859,11 +1893,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>-10.699999998697299</v>
       </c>
       <c r="C2">
@@ -1879,7 +1913,7 @@
         <v>114.48999997212221</v>
       </c>
       <c r="F2">
-        <f>(B2-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" ref="F2:F26" si="0">(B2-AVERAGE(B$2:B$26))^2</f>
         <v>2396.6899360357938</v>
       </c>
       <c r="G2">
@@ -1887,811 +1921,820 @@
         <v>11796.566543875842</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>13.684522746741299</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>15.6494878213382</v>
+      </c>
+      <c r="B3">
         <v>-38.2999999991804</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C26" si="0">(A3-B3)</f>
-        <v>51.984522745921701</v>
+        <f t="shared" ref="C3:C26" si="1">(A3-B3)</f>
+        <v>53.949487820518598</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D26" si="1">ABS(C3)</f>
-        <v>51.984522745921701</v>
+        <f t="shared" ref="D3:D26" si="2">ABS(C3)</f>
+        <v>53.949487820518598</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E26" si="2">C3*C3</f>
-        <v>2702.3906051212507</v>
+        <f t="shared" ref="E3:E26" si="3">C3*C3</f>
+        <v>2910.5472360962845</v>
       </c>
       <c r="F3">
-        <f>(B3-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>456.07873599498009</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G26" si="3">(ABS(A3-AVERAGE($B$2:$B$26))+ABS(B3-AVERAGE($B$2:$B$26)))^2</f>
-        <v>8967.4314201243469</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+        <f t="shared" ref="G3:G26" si="4">(ABS(A3-AVERAGE($B$2:$B$26))+ABS(B3-AVERAGE($B$2:$B$26)))^2</f>
+        <v>9343.4432276308235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>13.0893405284962</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>-55.699999998752297</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.789340527248498</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68.789340527248498</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4731.9733701737523</v>
       </c>
       <c r="F4">
-        <f>(B4-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>15.649936002457263</v>
       </c>
       <c r="G4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5883.0956387722163</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>13.281382672687499</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14.7448891462071</v>
+      </c>
+      <c r="B5">
         <v>-57.499999999343899</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>70.781382672031398</v>
+        <f t="shared" si="1"/>
+        <v>72.244889145550999</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>70.781382672031398</v>
+        <f t="shared" si="2"/>
+        <v>72.244889145550999</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>5010.0041329645464</v>
+        <f t="shared" si="3"/>
+        <v>5219.3240076529528</v>
       </c>
       <c r="F5">
-        <f>(B5-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>4.6483359987882071</v>
       </c>
       <c r="G5">
-        <f t="shared" si="3"/>
-        <v>5639.0161210437318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>12.040360120451499</v>
-      </c>
-      <c r="B6" s="1">
+        <f t="shared" si="4"/>
+        <v>5860.9572755581257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>15.6466964913062</v>
+      </c>
+      <c r="B6">
         <v>-60.299999998856897</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>72.3403601193084</v>
+        <f t="shared" si="1"/>
+        <v>75.946696490163092</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>72.3403601193084</v>
+        <f t="shared" si="2"/>
+        <v>75.946696490163092</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>5233.1277021912256</v>
+        <f t="shared" si="3"/>
+        <v>5767.9007077689512</v>
       </c>
       <c r="F6">
-        <f>(B6-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>0.41473599973470576</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
-        <v>5233.1277021912256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>16.546944111758599</v>
-      </c>
-      <c r="B7" s="1">
+        <f t="shared" si="4"/>
+        <v>5767.900707768953</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>21.5910927482043</v>
+      </c>
+      <c r="B7">
         <v>-67.899999999281505</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>84.446944111040096</v>
+        <f t="shared" si="1"/>
+        <v>89.491092747485808</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>84.446944111040096</v>
+        <f t="shared" si="2"/>
+        <v>89.491092747485808</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>7131.2863696931299</v>
+        <f t="shared" si="3"/>
+        <v>8008.6556811391074</v>
       </c>
       <c r="F7">
-        <f>(B7-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>67.96353600360483</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
-        <v>7131.2863696931317</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>6.8296693569677096</v>
-      </c>
-      <c r="B8" s="1">
+        <f t="shared" si="4"/>
+        <v>8008.6556811391074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9.1314260373540002</v>
+      </c>
+      <c r="B8">
         <v>-71.799999999375203</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>78.629669356342916</v>
+        <f t="shared" si="1"/>
+        <v>80.931426036729206</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>78.629669356342916</v>
+        <f t="shared" si="2"/>
+        <v>80.931426036729206</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>6182.6249030878125</v>
+        <f t="shared" si="3"/>
+        <v>6549.8957203385698</v>
       </c>
       <c r="F8">
-        <f>(B8-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>147.47673600758591</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
-        <v>6182.6249030878125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>18.2981383951387</v>
-      </c>
-      <c r="B9" s="1">
+        <f t="shared" si="4"/>
+        <v>6549.8957203385698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>19.432721010301101</v>
+      </c>
+      <c r="B9">
         <v>-71.099999999010095</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>89.398138394148788</v>
+        <f t="shared" si="1"/>
+        <v>90.532721009311189</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>89.398138394148788</v>
+        <f t="shared" si="2"/>
+        <v>90.532721009311189</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>7992.0271483393799</v>
+        <f t="shared" si="3"/>
+        <v>8196.1735733497753</v>
       </c>
       <c r="F9">
-        <f>(B9-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>130.96513599879205</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
-        <v>7992.0271483393817</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>22.1225426696402</v>
-      </c>
-      <c r="B10" s="1">
+        <f t="shared" si="4"/>
+        <v>8196.173573349779</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>22.5216586248869</v>
+      </c>
+      <c r="B10">
         <v>-74.399999999247001</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>96.522542668887198</v>
+        <f t="shared" si="1"/>
+        <v>96.921658624133897</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>96.522542668887198</v>
+        <f t="shared" si="2"/>
+        <v>96.921658624133897</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>9316.6012432671505</v>
+        <f t="shared" si="3"/>
+        <v>9393.807910453148</v>
       </c>
       <c r="F10">
-        <f>(B10-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>217.38553600542963</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
-        <v>9316.6012432671505</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>12.8066560959927</v>
-      </c>
-      <c r="B11" s="1">
+        <f t="shared" si="4"/>
+        <v>9393.807910453148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>13.283504509425301</v>
+      </c>
+      <c r="B11">
         <v>-81.699999998636002</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>94.50665609462871</v>
+        <f t="shared" si="1"/>
+        <v>94.983504508061301</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>94.50665609462871</v>
+        <f t="shared" si="2"/>
+        <v>94.983504508061301</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>8931.5080461884227</v>
+        <f t="shared" si="3"/>
+        <v>9021.8661286329025</v>
       </c>
       <c r="F11">
-        <f>(B11-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>485.9379359811802</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
-        <v>8931.508046188419</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>24.562731439754501</v>
-      </c>
-      <c r="B12" s="1">
+        <f t="shared" si="4"/>
+        <v>9021.8661286329025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>24.951864233187901</v>
+      </c>
+      <c r="B12">
         <v>-81.999999999245404</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>106.5627314389999</v>
+        <f t="shared" si="1"/>
+        <v>106.95186423243331</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>106.5627314389999</v>
+        <f t="shared" si="2"/>
+        <v>106.95186423243331</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>11355.61573174042</v>
+        <f t="shared" si="3"/>
+        <v>11438.701262792847</v>
       </c>
       <c r="F12">
-        <f>(B12-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>499.254336008157</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
-        <v>11355.61573174042</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>21.269594282810299</v>
-      </c>
-      <c r="B13" s="1">
+        <f t="shared" si="4"/>
+        <v>11438.701262792847</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21.663315873935701</v>
+      </c>
+      <c r="B13">
         <v>-71.9999999983431</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>93.269594281153402</v>
+        <f t="shared" si="1"/>
+        <v>93.663315872278801</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>93.269594281153402</v>
+        <f t="shared" si="2"/>
+        <v>93.663315872278801</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
-        <v>8699.2172173709641</v>
+        <f t="shared" si="3"/>
+        <v>8772.8167401902738</v>
       </c>
       <c r="F13">
-        <f>(B13-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>152.37433598223029</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
-        <v>8699.2172173709641</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>17.4831133695061</v>
-      </c>
-      <c r="B14" s="1">
+        <f t="shared" si="4"/>
+        <v>8772.8167401902738</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>17.633116728369501</v>
+      </c>
+      <c r="B14">
         <v>-63.299999999521901</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>80.783113369028001</v>
+        <f t="shared" si="1"/>
+        <v>80.933116727891402</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>80.783113369028001</v>
+        <f t="shared" si="2"/>
+        <v>80.933116727891402</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
-        <v>6525.9114055932305</v>
+        <f t="shared" si="3"/>
+        <v>6550.1693832904948</v>
       </c>
       <c r="F14">
-        <f>(B14-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>13.278736003345413</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
-        <v>6525.9114055932305</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>15.8542831263943</v>
-      </c>
-      <c r="B15" s="1">
+        <f t="shared" si="4"/>
+        <v>6550.1693832904948</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15.8556917152879</v>
+      </c>
+      <c r="B15">
         <v>-63.599999999314399</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>79.454283125708699</v>
+        <f t="shared" si="1"/>
+        <v>79.455691714602295</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>79.454283125708699</v>
+        <f t="shared" si="2"/>
+        <v>79.455691714602295</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
-        <v>6312.9831070202781</v>
+        <f t="shared" si="3"/>
+        <v>6313.20694584592</v>
       </c>
       <c r="F15">
-        <f>(B15-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>15.555136001984049</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
-        <v>6312.9831070202754</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>20.0066875678922</v>
-      </c>
-      <c r="B16" s="1">
+        <f t="shared" si="4"/>
+        <v>6313.20694584592</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20.188900431782901</v>
+      </c>
+      <c r="B16">
         <v>-66.599999999403195</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>86.606687567295396</v>
+        <f t="shared" si="1"/>
+        <v>86.788900431186093</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>86.606687567295396</v>
+        <f t="shared" si="2"/>
+        <v>86.788900431186093</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
-        <v>7500.7183313791193</v>
+        <f t="shared" si="3"/>
+        <v>7532.3132380543339</v>
       </c>
       <c r="F16">
-        <f>(B16-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>48.219136004726423</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
-        <v>7500.7183313791193</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>17.21878422372</v>
-      </c>
-      <c r="B17" s="1">
+        <f t="shared" si="4"/>
+        <v>7532.3132380543339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17.152638564649799</v>
+      </c>
+      <c r="B17">
         <v>-76.799999999169501</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>94.018784222889508</v>
+        <f t="shared" si="1"/>
+        <v>93.952638563819306</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>94.018784222889508</v>
+        <f t="shared" si="2"/>
+        <v>93.952638563819306</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
-        <v>8839.5317867502563</v>
+        <f t="shared" si="3"/>
+        <v>8827.0982931036669</v>
       </c>
       <c r="F17">
-        <f>(B17-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>293.91673600365613</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
-        <v>8839.5317867502545</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>12.594250000000001</v>
-      </c>
-      <c r="B18" s="1">
+        <f t="shared" si="4"/>
+        <v>8827.0982931036633</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12.5793083442318</v>
+      </c>
+      <c r="B18">
         <v>-71.399999999576707</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>83.994249999576709</v>
+        <f t="shared" si="1"/>
+        <v>83.979308343808512</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>83.994249999576709</v>
+        <f t="shared" si="2"/>
+        <v>83.979308343808512</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
-        <v>7055.0340329913925</v>
+        <f t="shared" si="3"/>
+        <v>7052.5242299044658</v>
       </c>
       <c r="F18">
-        <f>(B18-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>137.92153601206897</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
-        <v>7055.0340329913925</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>16.554566004815101</v>
-      </c>
-      <c r="B19" s="1">
+        <f t="shared" si="4"/>
+        <v>7052.5242299044658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16.546550488609601</v>
+      </c>
+      <c r="B19">
         <v>-83.599999998864803</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>100.1545660036799</v>
+        <f t="shared" si="1"/>
+        <v>100.1465504874744</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>100.1545660036799</v>
+        <f t="shared" si="2"/>
+        <v>100.1465504874744</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
-        <v>10030.937091385475</v>
+        <f t="shared" si="3"/>
+        <v>10029.33157454026</v>
       </c>
       <c r="F19">
-        <f>(B19-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>573.31513599051493</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
-        <v>10030.937091385475</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>30.005727805739902</v>
-      </c>
-      <c r="B20" s="1">
+        <f t="shared" si="4"/>
+        <v>10029.33157454026</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>30.2881972794024</v>
+      </c>
+      <c r="B20">
         <v>-65.799999998663793</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>95.805727804403688</v>
+        <f t="shared" si="1"/>
+        <v>96.08819727806619</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
-        <v>95.805727804403688</v>
+        <f t="shared" si="2"/>
+        <v>96.08819727806619</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
-        <v>9178.7374801314891</v>
+        <f t="shared" si="3"/>
+        <v>9232.9416561485668</v>
       </c>
       <c r="F20">
-        <f>(B20-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>37.748735995096126</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
-        <v>9178.7374801314927</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>7.30497160240576</v>
-      </c>
-      <c r="B21" s="1">
+        <f t="shared" si="4"/>
+        <v>9232.9416561485668</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7.2509557459792404</v>
+      </c>
+      <c r="B21">
         <v>-88.699999999393398</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>96.004971601799156</v>
+        <f t="shared" si="1"/>
+        <v>95.950955745372639</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>96.004971601799156</v>
+        <f t="shared" si="2"/>
+        <v>95.950955745372639</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
-        <v>9216.9545722622624</v>
+        <f t="shared" si="3"/>
+        <v>9206.5859084504591</v>
       </c>
       <c r="F21">
-        <f>(B21-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>843.55393601919968</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
-        <v>9216.9545722622624</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>45.312769420289101</v>
-      </c>
-      <c r="B22" s="1">
+        <f t="shared" si="4"/>
+        <v>9206.5859084504591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>46.187126821272102</v>
+      </c>
+      <c r="B22">
         <v>-45.399999998297702</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>90.712769418586802</v>
+        <f t="shared" si="1"/>
+        <v>91.587126819569804</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
-        <v>90.712769418586802</v>
+        <f t="shared" si="2"/>
+        <v>91.587126819569804</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
-        <v>8228.8065355896979</v>
+        <f t="shared" si="3"/>
+        <v>8388.2017990639615</v>
       </c>
       <c r="F22">
-        <f>(B22-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>203.23353602181652</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
-        <v>14214.5456432801</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>54.870090874615798</v>
-      </c>
-      <c r="B23" s="1">
+        <f t="shared" si="4"/>
+        <v>14423.800263190695</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>56.491329067400102</v>
+      </c>
+      <c r="B23">
         <v>-55.799999999449099</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>110.6700908740649</v>
+        <f t="shared" si="1"/>
+        <v>112.2913290668492</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
-        <v>110.6700908740649</v>
+        <f t="shared" si="2"/>
+        <v>112.2913290668492</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
-        <v>12247.869014073782</v>
+        <f t="shared" si="3"/>
+        <v>12609.342583599413</v>
       </c>
       <c r="F23">
-        <f>(B23-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>14.868735997021409</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
-        <v>14014.31943953247</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>103.64004406186901</v>
-      </c>
-      <c r="B24" s="1">
+        <f t="shared" si="4"/>
+        <v>14400.798986941099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>105.779654445178</v>
+      </c>
+      <c r="B24">
         <v>-15.6999999989923</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>119.3400440608613</v>
+        <f t="shared" si="1"/>
+        <v>121.47965444417029</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
-        <v>119.3400440608613</v>
+        <f t="shared" si="2"/>
+        <v>121.47965444417029</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
-        <v>14242.046116448317</v>
+        <f t="shared" si="3"/>
+        <v>14757.306443875023</v>
       </c>
       <c r="F24">
-        <f>(B24-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1932.1299360062044</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
-        <v>42953.409767463694</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>111.133312213243</v>
-      </c>
-      <c r="B25" s="1">
+        <f t="shared" si="4"/>
+        <v>43844.864950925927</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>114.747292581568</v>
+      </c>
+      <c r="B25">
         <v>-23.099999998818799</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>134.2333122120618</v>
+        <f t="shared" si="1"/>
+        <v>137.84729258038681</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
-        <v>134.2333122120618</v>
+        <f t="shared" si="2"/>
+        <v>137.84729258038681</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
-        <v>18018.582107420862</v>
+        <f t="shared" si="3"/>
+        <v>19001.876071742765</v>
       </c>
       <c r="F25">
-        <f>(B25-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>1336.3411360178443</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
-        <v>42992.078496519811</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>119.23831221324301</v>
-      </c>
-      <c r="B26" s="1">
+        <f t="shared" si="4"/>
+        <v>44503.8231262232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>122.857960757832</v>
+      </c>
+      <c r="B26">
         <v>-28.1999999991374</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>147.4383122123804</v>
+        <f t="shared" si="1"/>
+        <v>151.05796075696941</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
-        <v>147.4383122123804</v>
+        <f t="shared" si="2"/>
+        <v>151.05796075696941</v>
       </c>
       <c r="E26">
-        <f t="shared" si="2"/>
-        <v>21738.05590803536</v>
+        <f t="shared" si="3"/>
+        <v>22818.50750805411</v>
       </c>
       <c r="F26">
-        <f>(B26-AVERAGE(B$2:B$26))^2</f>
+        <f t="shared" si="0"/>
         <v>989.47993599531117</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
-        <v>44247.253847783199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>45783.144106275235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
         <f>SUM(C2:C26)</f>
-        <v>2237.1487948807448</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2266.6647199727781</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30">
         <f>SUM(C2:C26)/AVERAGE(B2:B26)</f>
-        <v>-37.500817938109961</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-37.995586697203713</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31">
         <f>SUM(C2:C26)/AVERAGE(B2:B26)*100</f>
-        <v>-3750.0817938109963</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-3799.5586697203712</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32" cm="1">
         <f t="array" ref="B32">MAX(ABS(C2:C26))</f>
-        <v>147.4383122123804</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>151.05796075696941</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
       <c r="B33">
         <f>AVERAGE(C2:C26)</f>
-        <v>89.485951795229795</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>90.666588798911121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34">
         <f>AVERAGE(D2:D26)</f>
-        <v>89.485951795229795</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>90.666588798911121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
       <c r="B35">
         <f>SUM(E2:E26)</f>
-        <v>216537.03395919173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>222445.55797423414</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
       <c r="B36">
         <f>CORREL(A2:A26,B2:B26)</f>
-        <v>0.60739801792038761</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.61084189423440305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
       <c r="B37">
         <f>B36^2</f>
-        <v>0.36893235217361553</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.37312781975187365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
       <c r="B38">
         <f>SQRT(AVERAGE(E2:E26))</f>
-        <v>93.067079885250877</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>94.328268928086274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
       <c r="B39">
         <f>B38/AVERAGE(B2:B26)</f>
-        <v>-1.5600623556174209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-1.5812033815470039</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
       <c r="B40">
         <f>B39*100</f>
-        <v>-156.0062355617421</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-158.12033815470039</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
       <c r="B41">
         <f>(SUM(A2:A26)-SUM(B2:B26))/SUM(B2:B26)</f>
-        <v>-1.5000327175243982</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-1.5198234678881484</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
       <c r="B42">
         <f>1-SUM(E2:E26)/SUM(F2:F26)</f>
-        <v>-18.659446043575446</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-19.195882268580668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
       <c r="B43">
         <f>1-SUM(E2:E26)/SUM(G2:G26)</f>
-        <v>0.32376667353466815</v>
+        <v>0.32126288363615085</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44">
+        <f>1-SQRT((B36-1)^2+(STDEV(A2:A26)/STDEV(B2:B26)-1)^2+(AVERAGE(A2:A26)/AVERAGE(B2:B26)-1)^2)</f>
+        <v>-0.66753269816339089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>